<commit_message>
Arreglos generales en scripts de generación de siniestros
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroAP.xlsx
+++ b/SuraClaims/GeneracionSiniestroAP.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Sura - Claims\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7238DC2E-84C1-4063-964A-8B29C5B5B384}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,12 +81,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>ssurgwsoadev4.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>https://ssurgwsoadev4.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
-  </si>
-  <si>
     <t>aseguradosgw@gmail.com</t>
   </si>
   <si>
@@ -101,9 +96,6 @@
     <t>Invalidez Parcial Permanente (AT)</t>
   </si>
   <si>
-    <t>28/05/2022</t>
-  </si>
-  <si>
     <t>rherner</t>
   </si>
   <si>
@@ -114,12 +106,21 @@
   </si>
   <si>
     <t>29/10/2020</t>
+  </si>
+  <si>
+    <t>23/06/2022</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,11 +453,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,25 +520,25 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="4">
-        <v>12420005757</v>
+        <v>12112002068</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
@@ -546,19 +547,19 @@
         <v>32039201</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>21</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>23</v>
       </c>
       <c r="O2">
         <v>967</v>
@@ -566,13 +567,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -584,7 +585,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>9</v>
@@ -593,19 +594,19 @@
         <v>32039201</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>21</v>
-      </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" t="s">
-        <v>23</v>
       </c>
       <c r="O3">
         <v>967</v>
@@ -613,10 +614,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="J2" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{61638A75-B3E6-4A88-8C02-38715525F0BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Todas las generaciones mejoradas
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroAP.xlsx
+++ b/SuraClaims/GeneracionSiniestroAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9062407-F1CB-40B3-A67B-D3F7AC221349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693E95B9-AC7C-41AB-834E-A316A66465D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,16 +105,16 @@
     <t>29/10/2020</t>
   </si>
   <si>
-    <t>23/06/2022</t>
+    <t>NumeroCalle</t>
+  </si>
+  <si>
+    <t>19/03/2021</t>
   </si>
   <si>
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
   </si>
   <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
-  </si>
-  <si>
-    <t>NumeroCalle</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,15 +515,15 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -532,13 +532,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="4">
-        <v>12112002068</v>
+        <v>12112002080</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
@@ -617,9 +617,8 @@
     <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{61638A75-B3E6-4A88-8C02-38715525F0BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completar actividades para realizar pagos. Verificar pagos en CC y en SISE
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroAP.xlsx
+++ b/SuraClaims/GeneracionSiniestroAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693E95B9-AC7C-41AB-834E-A316A66465D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0BF95D-AA14-472E-9796-67745A281494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Usuario</t>
   </si>
@@ -102,19 +102,22 @@
     <t>https://i-preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t>29/10/2020</t>
-  </si>
-  <si>
     <t>NumeroCalle</t>
   </si>
   <si>
-    <t>19/03/2021</t>
-  </si>
-  <si>
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
   </si>
   <si>
     <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>12112001841</t>
+  </si>
+  <si>
+    <t>07/04/2021</t>
+  </si>
+  <si>
+    <t>29/04/2022</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,15 +518,15 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -532,13 +535,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="4">
-        <v>12112002080</v>
+        <v>12112002243</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
@@ -578,14 +581,14 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>12112001528</v>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
enviar y validar inspección
</commit_message>
<xml_diff>
--- a/SuraClaims/GeneracionSiniestroAP.xlsx
+++ b/SuraClaims/GeneracionSiniestroAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545B0900-B9D0-4B3C-A354-92E7B400B746}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F556DE-3337-4D2F-8390-8848B9581878}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,16 +111,16 @@
     <t>07/04/2021</t>
   </si>
   <si>
-    <t>26/04/2021</t>
-  </si>
-  <si>
-    <t>12112002294</t>
-  </si>
-  <si>
     <t>preproducciongestion.segurossura.com.ar</t>
   </si>
   <si>
     <t>https://preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>12112002368</t>
+  </si>
+  <si>
+    <t>19/05/2021</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,13 +538,13 @@
         <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
@@ -573,10 +573,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>

</xml_diff>